<commit_message>
Cambio en formato focos excel
</commit_message>
<xml_diff>
--- a/src/assets/FormatoFocos.xlsx
+++ b/src/assets/FormatoFocos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lortiz\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trabajo\ProyectosVue\Engine_vue\engine-vue\enginev2-vue\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAC645F3-E795-4A8A-B080-D32A608AD39C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F732812E-83CD-44AC-8636-8168080B3300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4EE1B09-1F83-4878-A2C3-A4FD9140E6EA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Nombre</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>02041-02046</t>
+  </si>
+  <si>
+    <t>Fecha_inicio</t>
+  </si>
+  <si>
+    <t>Fecha_fin</t>
+  </si>
+  <si>
+    <t>2021-11-26</t>
+  </si>
+  <si>
+    <t>2021-11-30</t>
   </si>
 </sst>
 </file>
@@ -81,9 +93,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80622BEB-B7DE-4090-875A-B4B75903CE31}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,7 +422,7 @@
     <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,8 +435,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -435,6 +454,12 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>